<commit_message>
Automatic upload, adding images.
</commit_message>
<xml_diff>
--- a/items_data/costco.xlsx
+++ b/items_data/costco.xlsx
@@ -460,10 +460,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="2:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -526,291 +526,475 @@
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="4">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Squishmallows 16" Plush</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Squishmallow</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>12.99</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>16"</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Multi</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734774.html</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="inlineStr">
-        <is>
-          <t>1603399.jpg</t>
-        </is>
-      </c>
-      <c r="I2" s="3" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>8011603391.jpg</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="4">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Squishmallows 20" Hello Kitty Sunglasses</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Hello Kitty Sunglasses</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>27.99</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>20"</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Squishmallows 16" Plush</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Squishmallow</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12.99</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16"</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Teal</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>https://www.costco.com/squishmallows-20%22-hello-kitty-sunglasses.product.100742307.html</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>1603305.jpg</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>7061603393.jpg</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Squishmallows 16" Plush</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Squishmallow</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>12.99</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>16"</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>Purple</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734774.html</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>4191603399.jpg</t>
-        </is>
-      </c>
-      <c r="I4" s="3" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>361603390.jpg</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="4">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Squishmallows 16" Plush</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Squishmallow</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>12.99</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>16"</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>Multi</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734774.html</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>7421603394.jpg</t>
-        </is>
-      </c>
-      <c r="I5" s="3" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>4401603392.jpg</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
     <row r="6" ht="12.8" customHeight="1" s="4">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Squishmallows 16" Plush</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Squishmallow</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>12.99</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>16"</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>Pink</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Multi</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734774.html</t>
-        </is>
-      </c>
-      <c r="H6" s="3" t="inlineStr">
-        <is>
-          <t>6781603397.jpg</t>
-        </is>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>3541603391.jpg</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
     <row r="7" ht="12.8" customHeight="1" s="4">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Squishmallows 16" Plush</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Squishmallow</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12.99</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>16"</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Teal</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>5221603393.jpg</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Costco</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="4">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Squishmallows 16" Plush</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Squishmallow</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>12.99</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>16"</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>8231603390.jpg</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Costco</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="4">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Squishmallows 16" Plush</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Squishmallow</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12.99</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>16"</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-16%22-plush.product.100734711.html</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>6141603392.jpg</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Costco</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="4">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Squishmallows 20" Hello Kitty Sunglasses</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Hello Kitty Sunglasses</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>27.99</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>20"</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.costco.com/squishmallows-20%22-hello-kitty-sunglasses.product.100742307.html</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>1603305.jpg</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Costco</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="4">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Squishmallows 20” Star Wars Chewbacca Plush</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Squishmallows 20” Star Wars Chewbacca Plush</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squishmallows 20” Star Wars Chewbacca </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>27.99</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>https://www.costco.com/squishmallows-20%e2%80%9d-star-wars-chewbacca-plush.product.100691777.html</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>1545490.jpg</t>
         </is>
       </c>
-      <c r="I7" s="3" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Costco</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="4"/>
-    <row r="9" ht="12.8" customHeight="1" s="4"/>
-    <row r="10" ht="12.8" customHeight="1" s="4"/>
-    <row r="11" ht="12.8" customHeight="1" s="4"/>
     <row r="12" ht="12.8" customHeight="1" s="4"/>
     <row r="13" ht="12.8" customHeight="1" s="4"/>
     <row r="14" ht="12.8" customHeight="1" s="4"/>

</xml_diff>